<commit_message>
Monster Rewards - Added gold and xp gain for killed monsters back in
</commit_message>
<xml_diff>
--- a/data/content/Monsters.xlsx
+++ b/data/content/Monsters.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
+    <workbookView xWindow="1050" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterRarity" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -193,6 +198,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -241,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,7 +284,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -694,10 +702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,7 +714,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -731,8 +739,14 @@
       <c r="H1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -754,8 +768,14 @@
       <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -777,8 +797,14 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -800,8 +826,14 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -823,8 +855,14 @@
       <c r="H5">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -846,8 +884,14 @@
       <c r="H6">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -869,8 +913,14 @@
       <c r="H7">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -892,8 +942,14 @@
       <c r="H8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -914,6 +970,12 @@
       </c>
       <c r="H9">
         <v>0.8</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>